<commit_message>
Added batch files, edited countrysets Excel sheet in line with prior fix for issue #21
</commit_message>
<xml_diff>
--- a/batch/countrysets.xlsx
+++ b/batch/countrysets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Australia_Oceania" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="253">
   <si>
     <t>id</t>
   </si>
@@ -1440,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C52" sqref="C2:C52"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1488,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C52" si="0">C3&amp;" "&amp;B4</f>
+        <f t="shared" ref="C4:C53" si="0">C3&amp;" "&amp;B4</f>
         <v>ALB AND AUT</v>
       </c>
     </row>
@@ -2066,6 +2066,18 @@
       <c r="C52" t="str">
         <f t="shared" si="0"/>
         <v>ALB AND AUT BLR BEL BIH BGR HRV CZE DNK EST FRO FIN FRA DEU GRC GGY HUN ISL IRL IMN ITA JEY XKO LVA LIE LTU LUX MLT MDA MCO MNE NLD MKD NOR POL PRT ROU RUS SMR SRB SVK SVN ESP SJM SWE CHE UKR GBR VAT ALA</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>ALB AND AUT BLR BEL BIH BGR HRV CZE DNK EST FRO FIN FRA DEU GRC GGY HUN ISL IRL IMN ITA JEY XKO LVA LIE LTU LUX MLT MDA MCO MNE NLD MKD NOR POL PRT ROU RUS SMR SRB SVK SVN ESP SJM SWE CHE UKR GBR VAT ALA TUR</v>
       </c>
     </row>
   </sheetData>
@@ -2077,7 +2089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -2705,74 +2717,74 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR TKM</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM ARE</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR TKM ARE</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM ARE UZB</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR TKM ARE UZB</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM ARE UZB VNM</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR TKM ARE UZB VNM</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM ARE UZB VNM YEM</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TUR TKM ARE UZB VNM YEM</v>
+        <v>AFG XAD ARM AZE BHR BGD BTN IOT BRN KHM XCA Z03 CXR CCK CYP GEO Z07 IDN IRN IRQ ISR JPN JOR KAZ KWT KGZ LAO LBN MYS MDV MNG MMR NPL PRK ZNC OMN Z06 PSE XPI PHL QAT SAU SGP KOR XSP LKA SYR TWN TJK THA TLS TKM ARE UZB VNM YEM RUS</v>
       </c>
     </row>
   </sheetData>
@@ -2784,7 +2796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
@@ -3573,7 +3585,7 @@
         <v>199</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C61" si="0">C3&amp;" "&amp;B4</f>
+        <f t="shared" ref="C4:C39" si="0">C3&amp;" "&amp;B4</f>
         <v>AIA ATG BHS</v>
       </c>
     </row>

</xml_diff>